<commit_message>
updated solver fidelity options
</commit_message>
<xml_diff>
--- a/examples/1_optimizations_of_ref_vehicle/multirotor/validation.xlsx
+++ b/examples/1_optimizations_of_ref_vehicle/multirotor/validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/examples/1_optimizations_of_ref_vehicle/multirotor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5DFACE-01FF-7B46-AD68-A2F0AAC728C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C604E5-6A63-E24D-986A-59EE01558453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15320" yWindow="740" windowWidth="14920" windowHeight="18900" activeTab="3" xr2:uid="{843CD013-835A-1741-B375-CD508AE79BD2}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{843CD013-835A-1741-B375-CD508AE79BD2}"/>
   </bookViews>
   <sheets>
     <sheet name="multirotor_ref" sheetId="13" r:id="rId1"/>
@@ -717,18 +717,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -736,6 +727,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10150,8 +10150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CE37D87-B951-4841-B7CA-13CC46090773}">
   <dimension ref="B1:AO56"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10195,11 +10195,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="2:41" x14ac:dyDescent="0.2">
       <c r="U2" s="16" t="s">
@@ -10210,26 +10210,26 @@
       </c>
     </row>
     <row r="3" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="28" t="s">
         <v>118</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="28" t="s">
         <v>80</v>
       </c>
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="N3" s="27" t="s">
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="N3" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
       <c r="U3" s="7" t="s">
         <v>41</v>
       </c>
@@ -10629,11 +10629,11 @@
       <c r="H7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
       <c r="N7" s="6" t="s">
         <v>159</v>
       </c>
@@ -11065,11 +11065,11 @@
       <c r="H11" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="J11" s="30" t="s">
+      <c r="J11" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
       <c r="U11" s="2">
         <v>7</v>
       </c>
@@ -11147,11 +11147,11 @@
       </c>
     </row>
     <row r="12" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
       <c r="F12" s="24" t="s">
         <v>82</v>
       </c>
@@ -11172,11 +11172,11 @@
       <c r="L12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="30" t="s">
+      <c r="N12" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
       <c r="U12" s="2">
         <v>8</v>
       </c>
@@ -11371,7 +11371,7 @@
       <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="28" t="s">
         <v>86</v>
       </c>
       <c r="G14" s="31"/>
@@ -11593,11 +11593,11 @@
       <c r="L16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N16" s="30" t="s">
+      <c r="N16" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
       <c r="U16" s="2">
         <v>12</v>
       </c>
@@ -11675,11 +11675,11 @@
       </c>
     </row>
     <row r="17" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
       <c r="F17" s="6" t="s">
         <v>124</v>
       </c>
@@ -12441,12 +12441,12 @@
       </c>
     </row>
     <row r="24" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="F24" s="30" t="s">
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="F24" s="28" t="s">
         <v>81</v>
       </c>
       <c r="G24" s="31"/>
@@ -12985,11 +12985,11 @@
       </c>
     </row>
     <row r="29" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
       <c r="F29" t="s">
         <v>97</v>
       </c>
@@ -13093,11 +13093,11 @@
       <c r="H30" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="J30" s="27" t="s">
+      <c r="J30" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
       <c r="U30" s="2">
         <v>26</v>
       </c>
@@ -13383,7 +13383,7 @@
         <v>0.80011066800000008</v>
       </c>
       <c r="D33"/>
-      <c r="F33" s="30" t="s">
+      <c r="F33" s="28" t="s">
         <v>156</v>
       </c>
       <c r="G33" s="31"/>
@@ -13572,11 +13572,11 @@
       </c>
     </row>
     <row r="35" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
       <c r="F35" s="26" t="s">
         <v>132</v>
       </c>
@@ -13742,11 +13742,11 @@
       <c r="C38" s="17">
         <v>0.8</v>
       </c>
-      <c r="J38" s="27" t="s">
+      <c r="J38" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
+      <c r="K38" s="32"/>
+      <c r="L38" s="32"/>
       <c r="AF38" s="2">
         <v>34</v>
       </c>
@@ -13833,11 +13833,11 @@
       </c>
     </row>
     <row r="40" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
       <c r="J40" s="11" t="s">
         <v>52</v>
       </c>
@@ -14142,16 +14142,16 @@
       </c>
     </row>
     <row r="46" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B46" s="27" t="s">
+      <c r="B46" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="J46" s="27" t="s">
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="J46" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
+      <c r="K46" s="32"/>
+      <c r="L46" s="32"/>
       <c r="N46" s="6" t="s">
         <v>153</v>
       </c>
@@ -14255,11 +14255,11 @@
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B52" s="27" t="s">
+      <c r="B52" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B53" s="6" t="s">
@@ -14295,6 +14295,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="J46:L46"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="F33:H33"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="N16:P16"/>
     <mergeCell ref="B1:D1"/>
@@ -14307,17 +14318,6 @@
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="N12:P12"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="F33:H33"/>
   </mergeCells>
   <conditionalFormatting sqref="K28">
     <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="FALSE">
@@ -14349,7 +14349,7 @@
   <dimension ref="B1:AO56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14393,11 +14393,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="2:41" x14ac:dyDescent="0.2">
       <c r="U2" s="16" t="s">
@@ -14408,26 +14408,26 @@
       </c>
     </row>
     <row r="3" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="28" t="s">
         <v>118</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="28" t="s">
         <v>80</v>
       </c>
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="N3" s="27" t="s">
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="N3" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
       <c r="U3" s="7" t="s">
         <v>41</v>
       </c>
@@ -14827,11 +14827,11 @@
       <c r="H7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
       <c r="N7" s="6" t="s">
         <v>159</v>
       </c>
@@ -15263,11 +15263,11 @@
       <c r="H11" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="J11" s="30" t="s">
+      <c r="J11" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
       <c r="U11" s="2">
         <v>7</v>
       </c>
@@ -15345,11 +15345,11 @@
       </c>
     </row>
     <row r="12" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
       <c r="F12" s="24" t="s">
         <v>82</v>
       </c>
@@ -15370,11 +15370,11 @@
       <c r="L12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="30" t="s">
+      <c r="N12" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
       <c r="U12" s="2">
         <v>8</v>
       </c>
@@ -15569,7 +15569,7 @@
       <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="28" t="s">
         <v>86</v>
       </c>
       <c r="G14" s="31"/>
@@ -15791,11 +15791,11 @@
       <c r="L16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N16" s="30" t="s">
+      <c r="N16" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
       <c r="U16" s="2">
         <v>12</v>
       </c>
@@ -15873,11 +15873,11 @@
       </c>
     </row>
     <row r="17" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
       <c r="F17" s="6" t="s">
         <v>124</v>
       </c>
@@ -16639,12 +16639,12 @@
       </c>
     </row>
     <row r="24" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="F24" s="30" t="s">
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="F24" s="28" t="s">
         <v>81</v>
       </c>
       <c r="G24" s="31"/>
@@ -17183,11 +17183,11 @@
       </c>
     </row>
     <row r="29" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
       <c r="F29" t="s">
         <v>97</v>
       </c>
@@ -17291,11 +17291,11 @@
       <c r="H30" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="J30" s="27" t="s">
+      <c r="J30" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
       <c r="U30" s="2">
         <v>26</v>
       </c>
@@ -17581,7 +17581,7 @@
         <v>0.80011066800000008</v>
       </c>
       <c r="D33"/>
-      <c r="F33" s="30" t="s">
+      <c r="F33" s="28" t="s">
         <v>156</v>
       </c>
       <c r="G33" s="31"/>
@@ -17770,11 +17770,11 @@
       </c>
     </row>
     <row r="35" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
       <c r="F35" s="26" t="s">
         <v>132</v>
       </c>
@@ -17940,11 +17940,11 @@
       <c r="C38" s="17">
         <v>0.8</v>
       </c>
-      <c r="J38" s="27" t="s">
+      <c r="J38" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
+      <c r="K38" s="32"/>
+      <c r="L38" s="32"/>
       <c r="AF38" s="2">
         <v>34</v>
       </c>
@@ -18031,11 +18031,11 @@
       </c>
     </row>
     <row r="40" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
       <c r="J40" s="11" t="s">
         <v>52</v>
       </c>
@@ -18340,16 +18340,16 @@
       </c>
     </row>
     <row r="46" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B46" s="27" t="s">
+      <c r="B46" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="J46" s="27" t="s">
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="J46" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
+      <c r="K46" s="32"/>
+      <c r="L46" s="32"/>
       <c r="N46" s="6" t="s">
         <v>153</v>
       </c>
@@ -18453,11 +18453,11 @@
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B52" s="27" t="s">
+      <c r="B52" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B53" s="6" t="s">
@@ -18493,11 +18493,12 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="J46:L46"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="B12:D12"/>
@@ -18510,12 +18511,11 @@
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="J30:L30"/>
     <mergeCell ref="F33:H33"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="N3:P3"/>
   </mergeCells>
   <conditionalFormatting sqref="K28">
     <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="FALSE">
@@ -18547,7 +18547,7 @@
   <dimension ref="B1:AO56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18591,11 +18591,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="2:41" x14ac:dyDescent="0.2">
       <c r="U2" s="16" t="s">
@@ -18606,26 +18606,26 @@
       </c>
     </row>
     <row r="3" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="28" t="s">
         <v>118</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="28" t="s">
         <v>80</v>
       </c>
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="N3" s="27" t="s">
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="N3" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
       <c r="U3" s="7" t="s">
         <v>41</v>
       </c>
@@ -19025,11 +19025,11 @@
       <c r="H7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
       <c r="N7" s="6" t="s">
         <v>159</v>
       </c>
@@ -19461,11 +19461,11 @@
       <c r="H11" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="J11" s="30" t="s">
+      <c r="J11" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
       <c r="U11" s="2">
         <v>7</v>
       </c>
@@ -19543,11 +19543,11 @@
       </c>
     </row>
     <row r="12" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
       <c r="F12" s="24" t="s">
         <v>82</v>
       </c>
@@ -19568,11 +19568,11 @@
       <c r="L12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="30" t="s">
+      <c r="N12" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
       <c r="U12" s="2">
         <v>8</v>
       </c>
@@ -19767,7 +19767,7 @@
       <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="28" t="s">
         <v>86</v>
       </c>
       <c r="G14" s="31"/>
@@ -19989,11 +19989,11 @@
       <c r="L16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N16" s="30" t="s">
+      <c r="N16" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
       <c r="U16" s="2">
         <v>12</v>
       </c>
@@ -20071,11 +20071,11 @@
       </c>
     </row>
     <row r="17" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
       <c r="F17" s="6" t="s">
         <v>124</v>
       </c>
@@ -20837,12 +20837,12 @@
       </c>
     </row>
     <row r="24" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="F24" s="30" t="s">
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="F24" s="28" t="s">
         <v>81</v>
       </c>
       <c r="G24" s="31"/>
@@ -21381,11 +21381,11 @@
       </c>
     </row>
     <row r="29" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
       <c r="F29" t="s">
         <v>97</v>
       </c>
@@ -21489,11 +21489,11 @@
       <c r="H30" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="J30" s="27" t="s">
+      <c r="J30" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
       <c r="U30" s="2">
         <v>26</v>
       </c>
@@ -21779,7 +21779,7 @@
         <v>0.80011066800000008</v>
       </c>
       <c r="D33"/>
-      <c r="F33" s="30" t="s">
+      <c r="F33" s="28" t="s">
         <v>156</v>
       </c>
       <c r="G33" s="31"/>
@@ -21968,11 +21968,11 @@
       </c>
     </row>
     <row r="35" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
       <c r="F35" s="26" t="s">
         <v>132</v>
       </c>
@@ -22138,11 +22138,11 @@
       <c r="C38" s="17">
         <v>0.8</v>
       </c>
-      <c r="J38" s="27" t="s">
+      <c r="J38" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
+      <c r="K38" s="32"/>
+      <c r="L38" s="32"/>
       <c r="AF38" s="2">
         <v>34</v>
       </c>
@@ -22229,11 +22229,11 @@
       </c>
     </row>
     <row r="40" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
       <c r="J40" s="11" t="s">
         <v>52</v>
       </c>
@@ -22538,16 +22538,16 @@
       </c>
     </row>
     <row r="46" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B46" s="27" t="s">
+      <c r="B46" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="J46" s="27" t="s">
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="J46" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
+      <c r="K46" s="32"/>
+      <c r="L46" s="32"/>
       <c r="N46" s="6" t="s">
         <v>153</v>
       </c>
@@ -22651,11 +22651,11 @@
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B52" s="27" t="s">
+      <c r="B52" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B53" s="6" t="s">
@@ -22691,11 +22691,12 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="J46:L46"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="B12:D12"/>
@@ -22708,12 +22709,11 @@
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="J30:L30"/>
     <mergeCell ref="F33:H33"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="N3:P3"/>
   </mergeCells>
   <conditionalFormatting sqref="K28">
     <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="FALSE">
@@ -22789,11 +22789,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="2:41" x14ac:dyDescent="0.2">
       <c r="U2" s="16" t="s">
@@ -22804,26 +22804,26 @@
       </c>
     </row>
     <row r="3" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="28" t="s">
         <v>118</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="28" t="s">
         <v>80</v>
       </c>
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="N3" s="27" t="s">
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="N3" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
       <c r="U3" s="7" t="s">
         <v>41</v>
       </c>
@@ -23223,11 +23223,11 @@
       <c r="H7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
       <c r="N7" s="6" t="s">
         <v>159</v>
       </c>
@@ -23659,11 +23659,11 @@
       <c r="H11" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="J11" s="30" t="s">
+      <c r="J11" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
       <c r="U11" s="2">
         <v>7</v>
       </c>
@@ -23741,11 +23741,11 @@
       </c>
     </row>
     <row r="12" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
       <c r="F12" s="24" t="s">
         <v>82</v>
       </c>
@@ -23766,11 +23766,11 @@
       <c r="L12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="30" t="s">
+      <c r="N12" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
       <c r="U12" s="2">
         <v>8</v>
       </c>
@@ -23965,7 +23965,7 @@
       <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="28" t="s">
         <v>86</v>
       </c>
       <c r="G14" s="31"/>
@@ -24187,11 +24187,11 @@
       <c r="L16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N16" s="30" t="s">
+      <c r="N16" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
       <c r="U16" s="2">
         <v>12</v>
       </c>
@@ -24269,11 +24269,11 @@
       </c>
     </row>
     <row r="17" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
       <c r="F17" s="6" t="s">
         <v>124</v>
       </c>
@@ -25035,12 +25035,12 @@
       </c>
     </row>
     <row r="24" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="F24" s="30" t="s">
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="F24" s="28" t="s">
         <v>81</v>
       </c>
       <c r="G24" s="31"/>
@@ -25579,11 +25579,11 @@
       </c>
     </row>
     <row r="29" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
       <c r="F29" t="s">
         <v>97</v>
       </c>
@@ -25687,11 +25687,11 @@
       <c r="H30" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="J30" s="27" t="s">
+      <c r="J30" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
       <c r="U30" s="2">
         <v>26</v>
       </c>
@@ -25977,7 +25977,7 @@
         <v>0.80011066800000008</v>
       </c>
       <c r="D33"/>
-      <c r="F33" s="30" t="s">
+      <c r="F33" s="28" t="s">
         <v>156</v>
       </c>
       <c r="G33" s="31"/>
@@ -26166,11 +26166,11 @@
       </c>
     </row>
     <row r="35" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
       <c r="F35" s="26" t="s">
         <v>132</v>
       </c>
@@ -26336,11 +26336,11 @@
       <c r="C38" s="17">
         <v>0.8</v>
       </c>
-      <c r="J38" s="27" t="s">
+      <c r="J38" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
+      <c r="K38" s="32"/>
+      <c r="L38" s="32"/>
       <c r="AF38" s="2">
         <v>34</v>
       </c>
@@ -26427,11 +26427,11 @@
       </c>
     </row>
     <row r="40" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
       <c r="J40" s="11" t="s">
         <v>52</v>
       </c>
@@ -26736,16 +26736,16 @@
       </c>
     </row>
     <row r="46" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B46" s="27" t="s">
+      <c r="B46" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="J46" s="27" t="s">
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="J46" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
+      <c r="K46" s="32"/>
+      <c r="L46" s="32"/>
       <c r="N46" s="6" t="s">
         <v>153</v>
       </c>
@@ -26849,11 +26849,11 @@
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B52" s="27" t="s">
+      <c r="B52" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B53" s="6" t="s">
@@ -26889,11 +26889,12 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="J46:L46"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="B12:D12"/>
@@ -26906,12 +26907,11 @@
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="J30:L30"/>
     <mergeCell ref="F33:H33"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="N3:P3"/>
   </mergeCells>
   <conditionalFormatting sqref="K28">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="FALSE">

</xml_diff>